<commit_message>
Added hyperbolic time of flight (TOFHYPER.8xp)and elliptic time of flight (TOFELLIP.8xp)programs which requires semimajor axis, eccentricity, and at least one true anomaly.  Two true anomalies can be entered.  One in list 1 element 6 and one in list 2 element 6.  The code doesn't handle orbit transfers, so you only need to enter semimajor axis in list 1 element one and eccentricity in list 1 element 2.  Nothing else is needed in list 2.  See the variable map for more information.  There is not user querying so the values must be entered manually.
Added a flight path to orbital elements program.  The program requires radial distance, r, speed, v, and flight path angle (check your sign!).  This program is still WIP.
</commit_message>
<xml_diff>
--- a/AERE351_Astrodynamics_TI84_Variable_Map.xlsx
+++ b/AERE351_Astrodynamics_TI84_Variable_Map.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Orbital Elements" sheetId="1" r:id="rId1"/>
+    <sheet name="Time of Flight" sheetId="2" r:id="rId2"/>
+    <sheet name="Other" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="91">
   <si>
     <t>A</t>
   </si>
@@ -247,6 +247,48 @@
   </si>
   <si>
     <t>GC2PF</t>
+  </si>
+  <si>
+    <t>Orbital Elements 0</t>
+  </si>
+  <si>
+    <t>Orbital Elements 1</t>
+  </si>
+  <si>
+    <t>Eccentricity 0 (rad)</t>
+  </si>
+  <si>
+    <t>Eccentricity 1 (rad)</t>
+  </si>
+  <si>
+    <t>TOF 0 (seconds)</t>
+  </si>
+  <si>
+    <t>TOF 1 (seconds)</t>
+  </si>
+  <si>
+    <t>TOF Total (seconds)</t>
+  </si>
+  <si>
+    <t>Orbital Period (seconds)</t>
+  </si>
+  <si>
+    <t>Hyperbolic Time of Flight (TOFHYPER)</t>
+  </si>
+  <si>
+    <t>Elliptical Time of Flight (TOFELLIP)</t>
+  </si>
+  <si>
+    <t>Flight Path Angle to Orbital Elements (FP2ORBIT)</t>
+  </si>
+  <si>
+    <t>Flight Path Angle (degrees)</t>
+  </si>
+  <si>
+    <t>Specific Energy</t>
+  </si>
+  <si>
+    <t>Random {Rp, Ra, Vp, Va}</t>
   </si>
 </sst>
 </file>
@@ -314,10 +356,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,53 +684,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="H1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="O1" s="6" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="O1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="F2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="6"/>
       <c r="O2" s="2" t="s">
         <v>30</v>
       </c>
@@ -916,40 +958,46 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I11" s="3"/>
       <c r="J11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I12" s="3"/>
       <c r="J12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H13" t="s">
+      <c r="B13" s="3"/>
+      <c r="H13" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1134,24 +1182,772 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="H7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="H8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="H20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>